<commit_message>
create AssertUtil, using Assert to compare the result
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase_v9.xlsx
+++ b/src/test/resources/TestCase_v9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaa./Documents/project/apiAuto/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{4CF87ACB-3065-AA4C-91E3-200CC18AF9CA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
+  <xr:revisionPtr documentId="13_ncr:1_{EF4875AA-FB6F-8241-85CA-68C3A6D051AF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
     <workbookView activeTab="1" windowHeight="16540" windowWidth="27440" xWindow="1360" xr2:uid="{2EB20F32-45DC-094A-B138-EAFCA248D3EC}" yWindow="1460"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>CaseId(用例编号)</t>
   </si>
@@ -108,9 +108,6 @@
     <t>{"mobilephone":"18813989003","pwd":"123456"}</t>
   </si>
   <si>
-    <t>{"status":0,"code":"20111","data":null,"msg":"用户名或者密码错误"}</t>
-  </si>
-  <si>
     <t>不满足条件的密码</t>
   </si>
   <si>
@@ -297,13 +294,10 @@
     <t>{"mobilephone":"18813989107","pwd":"123456"}</t>
   </si>
   <si>
+    <t>{"status":0,"code":"20111","data":null,"msg":"用户名或密码错误"}</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>{"status":0,"code":"20116","data":null,"msg":"输入金额的金额小数不能超过两位"}</t>
-  </si>
-  <si>
-    <t>{"status":1,"code":"10001","data":{"id":360,"regname":"小蜜蜂","pwd":"E10ADC3949BA59ABBE56E057F20F883E","mobilephone":"18813989007","leaveamount":"30000.00","type":"1","regtime":"2019-10-06 09:54:57.0"},"msg":"充值成功"}</t>
   </si>
 </sst>
 </file>
@@ -311,7 +305,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,12 +319,6 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -363,9 +351,6 @@
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -690,208 +675,208 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.1640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="25.1640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="18.83203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="77.1640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="22.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="77.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -903,21 +888,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00AAF4D-AF41-AD47-9EED-4A471AC20EBF}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="24.83203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="35.1640625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="55.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="79.1640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="57.1640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="55.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="79.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="73.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,10 +919,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -950,11 +935,14 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -967,11 +955,14 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -984,11 +975,14 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1001,11 +995,14 @@
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1021,8 +1018,11 @@
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1035,11 +1035,14 @@
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1052,11 +1055,14 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1069,11 +1075,14 @@
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1086,11 +1095,14 @@
       <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1098,16 +1110,19 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1115,16 +1130,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1132,19 +1150,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1152,19 +1167,16 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1172,19 +1184,16 @@
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1192,19 +1201,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1212,19 +1218,16 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1232,19 +1235,16 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1252,19 +1252,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1272,19 +1269,16 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1292,16 +1286,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>